<commit_message>
Inicio paper formato IEEE
</commit_message>
<xml_diff>
--- a/articles/Ficha de leitura.xlsx
+++ b/articles/Ficha de leitura.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="8610" activeTab="2"/>
+    <workbookView windowWidth="10140" windowHeight="8250" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131">
   <si>
     <t>Palavras-chave</t>
   </si>
@@ -270,6 +270,9 @@
     <t>Propõe um modelo de TS em que a distribuição do erro \varepsilon_t é estimado através de regressão quantílica. Utiliza como principal motivação problemas em que há heterogeneidade</t>
   </si>
   <si>
+    <t>Autoregression with non-gaussian innovations</t>
+  </si>
+  <si>
     <t>Definição da RQ Condicional Multivariada, em que há dependencia entre as variáveis aleatórias que se calculam os quantis</t>
   </si>
   <si>
@@ -331,6 +334,22 @@
   </si>
   <si>
     <t>Foco na estimação e avaliação de quantis específicos, para aplicações de VAR. Propõe novo teste de cobertura</t>
+  </si>
+  <si>
+    <t>Khosravi e Nahavandi</t>
+  </si>
+  <si>
+    <t>Combined Nonparametric Prediction Intervals for
+Wind Power Generation</t>
+  </si>
+  <si>
+    <t>Usan redes neurais para a determinação de múltiplos pontos de um intervalo de confiança como saída</t>
+  </si>
+  <si>
+    <t>Koenker</t>
+  </si>
+  <si>
+    <t>Quantile Autoregression</t>
   </si>
   <si>
     <t>Li e Zhu</t>
@@ -403,10 +422,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -440,7 +459,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -454,9 +473,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -470,33 +513,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -515,9 +549,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -531,16 +565,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,6 +579,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -560,26 +594,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -598,37 +617,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,7 +749,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,31 +785,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,97 +797,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,16 +811,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -840,6 +859,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -859,187 +908,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1049,17 +1068,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1131,9 +1147,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:P33" totalsRowShown="0">
-  <autoFilter ref="A1:P33"/>
-  <sortState ref="A1:P33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:P36" totalsRowShown="0">
+  <autoFilter ref="A1:P36"/>
+  <sortState ref="A1:P36">
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="16">
@@ -1163,7 +1179,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="4C4C4C"/>
+        <a:sysClr val="windowText" lastClr="363636"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1423,7 +1439,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1449,7 +1465,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -1654,32 +1670,32 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="4" width="5.375" customWidth="1"/>
+    <col min="2" max="4" width="5.37333333333333" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
     <col min="6" max="6" width="21.5" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="8.675" customWidth="1"/>
+    <col min="7" max="7" width="8.67333333333333" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.25" customWidth="1"/>
-    <col min="10" max="10" width="10.35" customWidth="1"/>
+    <col min="9" max="9" width="12.2533333333333" customWidth="1"/>
+    <col min="10" max="10" width="10.3533333333333" customWidth="1"/>
     <col min="11" max="11" width="13.5" customWidth="1"/>
-    <col min="12" max="13" width="8.375" customWidth="1"/>
-    <col min="14" max="14" width="40.875" customWidth="1"/>
+    <col min="12" max="13" width="8.37333333333333" customWidth="1"/>
+    <col min="14" max="14" width="40.8733333333333" customWidth="1"/>
     <col min="15" max="15" width="26.5" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="40.5" spans="1:16">
+    <row r="1" ht="38.25" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1729,7 +1745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="40.5" spans="1:16">
+    <row r="2" ht="38.25" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1759,7 +1775,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" ht="40.5" spans="1:14">
+    <row r="3" ht="38.25" spans="1:14">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1779,7 +1795,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" ht="40.5" spans="1:16">
+    <row r="4" ht="38.25" spans="1:16">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -1811,7 +1827,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" ht="40.5" spans="1:16">
+    <row r="5" ht="38.25" spans="1:16">
       <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
@@ -1843,7 +1859,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" ht="40.5" spans="1:16">
+    <row r="6" ht="38.25" spans="1:16">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -1877,7 +1893,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" ht="40.5" spans="1:16">
+    <row r="7" ht="25.5" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>68</v>
       </c>
@@ -1911,7 +1927,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" ht="67.5" spans="1:17">
+    <row r="8" ht="63.75" spans="1:16">
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
@@ -1931,14 +1947,13 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>75</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" ht="40.5" spans="1:16">
+    </row>
+    <row r="9" ht="38.25" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
@@ -1970,7 +1985,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" ht="67.5" spans="1:16">
+    <row r="10" ht="51" spans="1:16">
       <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
@@ -2004,41 +2019,33 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" ht="40.5" spans="1:16">
+    <row r="11" ht="25.5" spans="1:16">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1">
-        <v>2016</v>
+        <v>2009</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" ht="81" spans="1:16">
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" ht="38.25" spans="1:16">
       <c r="A12" s="1" t="s">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>2016</v>
@@ -2046,10 +2053,10 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -2057,272 +2064,280 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1">
-        <v>1</v>
-      </c>
+      <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" ht="54" spans="1:16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" ht="76.5" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="1">
-        <v>2009</v>
+        <v>2016</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G13" s="1">
         <v>1</v>
       </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
+      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="O13" s="1"/>
-      <c r="P13" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" ht="40.5" spans="1:16">
+      <c r="P13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" ht="51" spans="1:16">
       <c r="A14" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B14" s="1">
-        <v>2013</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>2009</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="1">
-        <v>1</v>
-      </c>
+      <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="P14" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" ht="27" spans="1:16">
+      <c r="P14" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" ht="38.25" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B15" s="1">
-        <v>2009</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>2013</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" ht="42" customHeight="1" spans="1:16">
+      <c r="P15" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" ht="25.5" spans="1:16">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B16" s="1">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" ht="40.5" spans="1:16">
+    <row r="17" ht="42" customHeight="1" spans="1:16">
       <c r="A17" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17" s="1">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G17" s="1">
         <v>1</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" ht="67.5" spans="1:16">
+    <row r="18" ht="38.25" spans="1:16">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="B18" s="1">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1">
         <v>1</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
+      <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" ht="63.75" spans="1:16">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1" t="s">
+      <c r="O19" s="1"/>
+      <c r="P19" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" ht="27" spans="1:14">
-      <c r="A19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B19">
-        <v>2008</v>
-      </c>
-      <c r="E19" t="s">
+    <row r="20" ht="38.25" spans="1:16">
+      <c r="A20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" ht="40.5" spans="1:16">
-      <c r="A20" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="B20" s="1">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1">
-        <v>1</v>
-      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1">
-        <v>1</v>
-      </c>
+      <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" ht="54" spans="1:16">
+    <row r="21" spans="1:16">
       <c r="A21" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" s="1">
-        <v>2015</v>
+        <v>2006</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1">
@@ -2330,65 +2345,57 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1">
-        <v>1</v>
-      </c>
+      <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" ht="54" spans="1:16">
-      <c r="A22" s="1" t="s">
+    <row r="22" ht="25.5" spans="1:14">
+      <c r="A22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22">
+        <v>2008</v>
+      </c>
+      <c r="E22" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="1">
-        <v>2013</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1">
-        <v>1</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-    </row>
-    <row r="23" spans="1:16">
+    </row>
+    <row r="23" ht="38.25" spans="1:16">
       <c r="A23" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B23" s="1">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -2396,21 +2403,19 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" ht="52" customHeight="1" spans="1:16">
+    <row r="24" ht="38.25" spans="1:16">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="B24" s="1">
-        <v>2005</v>
+        <v>2015</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="1">
         <v>1</v>
       </c>
@@ -2423,53 +2428,53 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" ht="54" spans="1:16">
+    <row r="25" ht="51" spans="1:16">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
       <c r="B25" s="1">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>38</v>
+        <v>118</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1">
         <v>1</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1">
-        <v>1</v>
-      </c>
-      <c r="J25" s="1"/>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" ht="67.5" spans="1:16">
+    <row r="26" spans="1:16">
       <c r="A26" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B26" s="1">
-        <v>2005</v>
+        <v>2011</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2478,48 +2483,58 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-      <c r="N26" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" ht="52" customHeight="1" spans="1:16">
       <c r="A27" s="1" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
+      <c r="N27" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" ht="27" spans="1:16">
+    <row r="28" ht="51" spans="1:16">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1">
-        <v>1991</v>
+        <v>2007</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1">
         <v>1</v>
@@ -2528,120 +2543,199 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
+      <c r="N28" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" ht="67.5" spans="1:11">
-      <c r="A29" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29">
-        <v>2016</v>
-      </c>
+    <row r="29" ht="63.75" spans="1:16">
+      <c r="A29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2005</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" ht="81" spans="1:16">
+        <v>122</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="1" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="B30" s="1">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-      <c r="H30" s="1">
-        <v>1</v>
-      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="N30" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" ht="54" spans="1:16">
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" ht="25.5" spans="1:16">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B31" s="1">
-        <v>2016</v>
+        <v>1991</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="1">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1">
         <v>1</v>
       </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="1">
-        <v>1</v>
-      </c>
+      <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-      <c r="N31" s="1" t="s">
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" ht="63.75" spans="1:11">
+      <c r="A32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32">
+        <v>2016</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" ht="76.5" spans="1:16">
+      <c r="A33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" ht="51" spans="1:16">
+      <c r="A34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1">
+        <v>1</v>
+      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1">
+        <v>1</v>
+      </c>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1" t="s">
+      <c r="O34" s="1"/>
+      <c r="P34" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" ht="40.5" spans="1:5">
-      <c r="A32" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32">
+    <row r="35" ht="38.25" spans="1:14">
+      <c r="A35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35">
         <v>2014</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" ht="40.5" spans="1:5">
-      <c r="A33" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33">
+      <c r="E35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" ht="38.25" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36">
         <v>2008</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>124</v>
+      <c r="E36" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit do dia 2017-07-05
</commit_message>
<xml_diff>
--- a/articles/Ficha de leitura.xlsx
+++ b/articles/Ficha de leitura.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10140" windowHeight="8250" activeTab="2"/>
+    <workbookView windowWidth="19020" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -425,10 +425,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -462,81 +462,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -554,14 +479,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -577,7 +510,68 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -590,11 +584,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -619,181 +619,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -817,6 +817,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -851,21 +866,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -909,142 +909,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -1172,7 +1172,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="363636"/>
+        <a:sysClr val="windowText" lastClr="4C4C4C"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1432,7 +1432,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1458,7 +1458,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -1668,27 +1668,27 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="4" width="5.37333333333333" customWidth="1"/>
+    <col min="2" max="4" width="5.375" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
     <col min="6" max="6" width="21.5" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="8.67333333333333" customWidth="1"/>
+    <col min="7" max="7" width="8.675" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.2533333333333" customWidth="1"/>
-    <col min="10" max="10" width="10.3533333333333" customWidth="1"/>
+    <col min="9" max="9" width="12.25" customWidth="1"/>
+    <col min="10" max="10" width="10.35" customWidth="1"/>
     <col min="11" max="11" width="13.5" customWidth="1"/>
-    <col min="12" max="13" width="8.37333333333333" customWidth="1"/>
-    <col min="14" max="14" width="40.8733333333333" customWidth="1"/>
+    <col min="12" max="13" width="8.375" customWidth="1"/>
+    <col min="14" max="14" width="40.875" customWidth="1"/>
     <col min="15" max="15" width="26.5" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="38.25" spans="1:16">
+    <row r="1" ht="40.5" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="38.25" spans="1:16">
+    <row r="2" ht="40.5" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" ht="38.25" spans="1:14">
+    <row r="3" ht="40.5" spans="1:14">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" ht="38.25" spans="1:16">
+    <row r="4" ht="40.5" spans="1:16">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" ht="38.25" spans="1:16">
+    <row r="5" ht="40.5" spans="1:16">
       <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
@@ -1852,7 +1852,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" ht="38.25" spans="1:16">
+    <row r="6" ht="40.5" spans="1:16">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" ht="25.5" spans="1:16">
+    <row r="7" ht="40.5" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>68</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" ht="63.75" spans="1:16">
+    <row r="8" ht="67.5" spans="1:16">
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
@@ -1948,7 +1948,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" ht="38.25" spans="1:16">
+    <row r="9" ht="40.5" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
@@ -1980,7 +1980,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" ht="51" spans="1:16">
+    <row r="10" ht="67.5" spans="1:16">
       <c r="A10" s="1" t="s">
         <v>80</v>
       </c>
@@ -2014,7 +2014,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" ht="25.5" spans="1:16">
+    <row r="11" ht="27" spans="1:16">
       <c r="A11" s="1" t="s">
         <v>80</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" ht="38.25" spans="1:16">
+    <row r="12" ht="40.5" spans="1:16">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" ht="76.5" spans="1:16">
+    <row r="13" ht="81" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" ht="51" spans="1:16">
+    <row r="14" ht="54" spans="1:16">
       <c r="A14" s="1" t="s">
         <v>87</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" ht="38.25" spans="1:16">
+    <row r="15" ht="40.5" spans="1:16">
       <c r="A15" s="1" t="s">
         <v>91</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" ht="25.5" spans="1:16">
+    <row r="16" ht="27" spans="1:16">
       <c r="A16" s="1" t="s">
         <v>97</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" ht="38.25" spans="1:16">
+    <row r="18" ht="40.5" spans="1:16">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
@@ -2262,7 +2262,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" ht="63.75" spans="1:16">
+    <row r="19" ht="67.5" spans="1:16">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" ht="38.25" spans="1:16">
+    <row r="20" ht="40.5" spans="1:16">
       <c r="A20" s="1" t="s">
         <v>106</v>
       </c>
@@ -2348,7 +2348,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" ht="25.5" spans="1:14">
+    <row r="22" ht="27" spans="1:14">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" ht="38.25" spans="1:16">
+    <row r="23" ht="40.5" spans="1:16">
       <c r="A23" s="1" t="s">
         <v>114</v>
       </c>
@@ -2398,7 +2398,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" ht="38.25" spans="1:16">
+    <row r="24" ht="54" spans="1:16">
       <c r="A24" s="1" t="s">
         <v>116</v>
       </c>
@@ -2428,7 +2428,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" ht="51" spans="1:16">
+    <row r="25" ht="54" spans="1:16">
       <c r="A25" s="1" t="s">
         <v>118</v>
       </c>
@@ -2514,7 +2514,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" ht="51" spans="1:16">
+    <row r="28" ht="54" spans="1:16">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -2546,7 +2546,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" ht="63.75" spans="1:16">
+    <row r="29" ht="67.5" spans="1:16">
       <c r="A29" s="1" t="s">
         <v>122</v>
       </c>
@@ -2596,7 +2596,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" ht="25.5" spans="1:16">
+    <row r="31" ht="27" spans="1:16">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -2622,7 +2622,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" ht="63.75" spans="1:11">
+    <row r="32" ht="67.5" spans="1:11">
       <c r="A32" t="s">
         <v>126</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" ht="76.5" spans="1:16">
+    <row r="33" ht="81" spans="1:16">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" ht="51" spans="1:16">
+    <row r="34" ht="54" spans="1:16">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" ht="38.25" spans="1:14">
+    <row r="35" ht="40.5" spans="1:14">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" ht="38.25" spans="1:5">
+    <row r="36" ht="40.5" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>130</v>
       </c>

</xml_diff>

<commit_message>
Commit do dia 18-09-17
</commit_message>
<xml_diff>
--- a/articles/Ficha de leitura.xlsx
+++ b/articles/Ficha de leitura.xlsx
@@ -3,8 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8670"/>
+    <workbookView windowWidth="10140" windowHeight="8160" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155">
   <si>
     <t>Autores</t>
   </si>
@@ -139,6 +140,16 @@
     <t>Cross-validation</t>
   </si>
   <si>
+    <t>Bergmeier, Hyndman e Koo</t>
+  </si>
+  <si>
+    <t>A Note on the Validity of Cross-Validation for Evaluating
+Autoregressive Time Series Prediction</t>
+  </si>
+  <si>
+    <t>Estimula o uso do K-fold CV para Time series, mesmo com valores futuros e selecionando diferentes valores de Lags</t>
+  </si>
+  <si>
     <t>Bertsimas e Mazumder</t>
   </si>
   <si>
@@ -163,7 +174,7 @@
     <t>Model Selection</t>
   </si>
   <si>
-    <t xml:space="preserve">Propõe a utilização de MILP para encontrar o melhor subconjunto </t>
+    <t>Propõe a utilização de MILP para encontrar o melhor subconjunto</t>
   </si>
   <si>
     <t>Parte quantílica não-paramétrica. Nossa estimação é diferente</t>
@@ -227,8 +238,7 @@
     <t>Gallego-Castillo, Bessa et al</t>
   </si>
   <si>
-    <t xml:space="preserve">On-line quantile regression in the RKHS (Reproducing Kernel Hilbert Space) for operational probabilistic forecasting of wind power
-</t>
+    <t>On-line quantile regression in the RKHS (Reproducing Kernel Hilbert Space) for operational probabilistic forecasting of wind power</t>
   </si>
   <si>
     <t>Wind Power, Quantile Regression</t>
@@ -318,7 +328,7 @@
     <t>Utilização de RQ para determinar a distribuição dos erros</t>
   </si>
   <si>
-    <t xml:space="preserve">Hastie, Tibshirani </t>
+    <t>Hastie, Tibshirani</t>
   </si>
   <si>
     <t>Extended Comparisons of Best Subset Selection, Forward Stepwise Selection, and the Lasso</t>
@@ -337,6 +347,15 @@
     <t>Usan redes neurais para a determinação de múltiplos pontos de um intervalo de confiança como saída</t>
   </si>
   <si>
+    <t>Koenker e Basset</t>
+  </si>
+  <si>
+    <t>Regression Quantiles</t>
+  </si>
+  <si>
+    <t>Artigo Seminal de Regressão Quantílica</t>
+  </si>
+  <si>
     <t>Koenker</t>
   </si>
   <si>
@@ -358,7 +377,7 @@
     <t>L1-norm Quantile Regression</t>
   </si>
   <si>
-    <t xml:space="preserve">Definem um algoritmo para a determinação do "regularization path" de forma mais eficiente. </t>
+    <t>Definem um algoritmo para a determinação do "regularization path" de forma mais eficiente.</t>
   </si>
   <si>
     <t>Li, Liu e Zhu</t>
@@ -425,8 +444,7 @@
     <t>Taieb, Huser, Hyndman e Genton</t>
   </si>
   <si>
-    <t xml:space="preserve">Forecasting Uncertainty in Electricity Smart Meter Data by Boosting Additive Quantile Regression
-</t>
+    <t>Forecasting Uncertainty in Electricity Smart Meter Data by Boosting Additive Quantile Regression</t>
   </si>
   <si>
     <t>Takeuchi e Le</t>
@@ -439,9 +457,6 @@
   </si>
   <si>
     <t>Motivação da restrição de non-crossing e estimação conjunta de todos os quantis. Utilização de uma função livre com penalização. No entanto, nós não utilizamos funções kernel</t>
-  </si>
-  <si>
-    <t>Taylor</t>
   </si>
   <si>
     <t>Wan et al.</t>
@@ -480,46 +495,35 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="24">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="2"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -532,92 +536,38 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color indexed="4"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="20"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -630,13 +580,104 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,200 +686,194 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="5"/>
-        <bgColor indexed="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor theme="6" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor theme="9" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor theme="7" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="26"/>
-        <bgColor indexed="26"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor theme="6" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor theme="4" tint="0.399975585192419"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor theme="4" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="47"/>
-        <bgColor indexed="47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor theme="5" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor theme="6" tint="0.399975585192419"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor theme="7" tint="0.399975585192419"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor theme="8" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor theme="8" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor theme="5" tint="0.799981688894314"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor theme="8" tint="0.399975585192419"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor theme="9" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor theme="9" tint="0.399975585192419"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -852,27 +887,30 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="1"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="1"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -881,7 +919,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -897,15 +935,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -951,11 +980,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -964,177 +999,161 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1193,41 +1212,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table3" displayName="Table3" ref="A1:Q45" totalsRowShown="0">
-  <autoFilter ref="A1:Q45"/>
-  <tableColumns count="17">
-    <tableColumn id="1" name="Autores"/>
-    <tableColumn id="2" name="Ano"/>
-    <tableColumn id="3" name="Citado"/>
-    <tableColumn id="4" name="Column1"/>
-    <tableColumn id="5" name="Nome do artigo"/>
-    <tableColumn id="6" name="Categorias"/>
-    <tableColumn id="7" name="QR"/>
-    <tableColumn id="8" name="QAR"/>
-    <tableColumn id="9" name="Empirical Distribution"/>
-    <tableColumn id="10" name="Functional Data"/>
-    <tableColumn id="11" name="Distribution-based TS"/>
-    <tableColumn id="12" name="Model identification"/>
-    <tableColumn id="13" name="Energy application"/>
-    <tableColumn id="14" name="MILP"/>
-    <tableColumn id="15" name="Resumo"/>
-    <tableColumn id="16" name="Comentários"/>
-    <tableColumn id="17" name="Pontos em comum com o nosso"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="363636"/>
+        <a:sysClr val="windowText" lastClr="212121"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="F3F3F3"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1263,13 +1256,73 @@
     <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1277,7 +1330,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1303,7 +1356,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1355,28 +1408,16 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1392,7 +1433,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1430,29 +1471,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="4" width="5.37333333333333" customWidth="1"/>
-    <col min="5" max="5" width="26.5" customWidth="1"/>
-    <col min="6" max="6" width="14.6333333333333" customWidth="1"/>
-    <col min="7" max="8" width="8.67333333333333" customWidth="1"/>
-    <col min="9" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="12.2533333333333" customWidth="1"/>
-    <col min="12" max="12" width="10.3533333333333" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
-    <col min="14" max="14" width="8.37333333333333" customWidth="1"/>
-    <col min="15" max="15" width="40.8733333333333" customWidth="1"/>
-    <col min="16" max="16" width="26.5" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5" customWidth="1"/>
+    <col min="1" max="1" width="26.675"/>
+    <col min="2" max="2" width="5.375"/>
+    <col min="3" max="4" width="5.35833333333333"/>
+    <col min="5" max="5" width="26.675"/>
+    <col min="6" max="6" width="14.7833333333333"/>
+    <col min="7" max="8" width="8.675"/>
+    <col min="9" max="10" width="12.1083333333333"/>
+    <col min="11" max="11" width="12.3166666666667"/>
+    <col min="12" max="12" width="10.3916666666667"/>
+    <col min="13" max="13" width="13.5"/>
+    <col min="14" max="14" width="8.35833333333333"/>
+    <col min="15" max="15" width="41.2416666666667"/>
+    <col min="16" max="16" width="9" hidden="1"/>
+    <col min="17" max="17" width="26.675"/>
   </cols>
   <sheetData>
     <row r="1" ht="38.25" spans="1:17">
@@ -1637,7 +1679,7 @@
       <c r="B6">
         <v>2017</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G6">
@@ -1657,170 +1699,154 @@
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" ht="25.5" spans="1:6">
+    <row r="8" ht="38.25" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="3">
         <v>2012</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" ht="38.25" spans="1:17">
-      <c r="A9" s="1" t="s">
+    <row r="9" ht="51" spans="1:15">
+      <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="3">
+        <v>2017</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1">
-        <v>1</v>
-      </c>
-      <c r="O9" s="1" t="s">
+    </row>
+    <row r="10" ht="38.25" spans="1:17">
+      <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" ht="25.5" spans="1:17">
-      <c r="A10" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="B10" s="1">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1">
-        <v>1</v>
-      </c>
+      <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1">
         <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" ht="63.75" spans="1:17">
-      <c r="A11" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" ht="38.25" spans="1:17">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B11" s="1">
-        <v>2004</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>2015</v>
+      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="7" t="s">
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" ht="63.75" spans="1:17">
+      <c r="A12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" ht="38.25" spans="1:17">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1">
+        <v>2004</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="1">
-        <v>1995</v>
-      </c>
-      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1">
-        <v>1</v>
-      </c>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="1" t="s">
-        <v>57</v>
+      <c r="O12" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" ht="51" spans="1:17">
+    <row r="13" ht="38.25" spans="1:17">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -1830,61 +1856,65 @@
         <v>1</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="1">
-        <v>1</v>
-      </c>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" ht="25.5" spans="1:17">
+    <row r="14" ht="51" spans="1:17">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1">
-        <v>2009</v>
+        <v>2002</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+      <c r="O14" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" ht="38.25" spans="1:17">
+    <row r="15" ht="25.5" spans="1:17">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1">
-        <v>2016</v>
+        <v>2009</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1892,17 +1922,13 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="1" t="s">
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" ht="38.25" spans="1:17">
+      <c r="A16" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" ht="76.5" spans="1:17">
-      <c r="A16" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="B16" s="1">
         <v>2016</v>
@@ -1910,10 +1936,10 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -1923,141 +1949,139 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1">
-        <v>1</v>
-      </c>
+      <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" ht="51" spans="1:17">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" ht="63.75" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1">
-        <v>2009</v>
+        <v>2016</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="G17" s="1">
         <v>1</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="1">
-        <v>1</v>
-      </c>
+      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="8" t="s">
+    </row>
+    <row r="18" ht="51" spans="1:17">
+      <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="18" ht="38.25" spans="1:17">
-      <c r="A18" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="B18" s="1">
-        <v>2013</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>2009</v>
+      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1">
         <v>1</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1">
-        <v>1</v>
-      </c>
+      <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" ht="38.25" spans="1:17">
+      <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2013</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" ht="25.5" spans="1:17">
-      <c r="A19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" s="1">
-        <v>2009</v>
-      </c>
-      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-    </row>
-    <row r="20" ht="42" customHeight="1" spans="1:17">
+    </row>
+    <row r="20" ht="25.5" spans="1:17">
       <c r="A20" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B20" s="1">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="1">
-        <v>1</v>
-      </c>
+      <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="1">
-        <v>1</v>
-      </c>
+      <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -2067,19 +2091,21 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" ht="38.25" spans="1:17">
+    <row r="21" ht="42" customHeight="1" spans="1:17">
       <c r="A21" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B21" s="1">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G21" s="1">
         <v>1</v>
       </c>
@@ -2088,7 +2114,9 @@
         <v>1</v>
       </c>
       <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -2098,12 +2126,12 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" ht="51" spans="1:17">
+    <row r="22" ht="38.25" spans="1:17">
       <c r="A22" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B22" s="1">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2114,91 +2142,91 @@
       <c r="G22" s="1">
         <v>1</v>
       </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+      <c r="O22" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" ht="63.75" spans="1:17">
+    <row r="23" ht="51" spans="1:17">
       <c r="A23" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="1">
         <v>1</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="M23" s="1"/>
       <c r="N23" s="1"/>
-      <c r="O23" s="1" t="s">
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" ht="63.75" spans="1:17">
+      <c r="A24" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" ht="51" spans="1:17">
-      <c r="A24" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="B24" s="1">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1">
-        <v>1</v>
-      </c>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1">
-        <v>1</v>
-      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N24" s="1"/>
       <c r="O24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-    </row>
-    <row r="25" ht="38.25" spans="1:17">
+    </row>
+    <row r="25" ht="51" spans="1:17">
       <c r="A25" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B25" s="1">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2211,21 +2239,25 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
       <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="N25" s="1">
+        <v>1</v>
+      </c>
       <c r="O25" s="1" t="s">
         <v>104</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" ht="38.25" spans="1:17">
       <c r="A26" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B26" s="1">
-        <v>2006</v>
+        <v>2013</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2233,9 +2265,7 @@
         <v>106</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
+      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2249,118 +2279,120 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" ht="38.25" spans="1:5">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:17">
+      <c r="A27" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
+        <v>1978</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="1">
         <v>2006</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" ht="25.5" spans="1:15">
-      <c r="A28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" ht="38.25" spans="1:5">
+      <c r="A29" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29">
+        <v>2006</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" ht="25.5" spans="1:15">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30">
         <v>2008</v>
       </c>
-      <c r="E28" t="s">
-        <v>111</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" ht="38.25" spans="1:17">
-      <c r="A29" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="1">
+      <c r="E30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" ht="38.25" spans="1:17">
+      <c r="A31" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="1">
         <v>2007</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1">
-        <v>1</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1">
-        <v>1</v>
-      </c>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1">
-        <v>1</v>
-      </c>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-    </row>
-    <row r="30" ht="38.25" spans="1:17">
-      <c r="A30" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B30" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1">
-        <v>1</v>
-      </c>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-    </row>
-    <row r="31" ht="25.5" spans="1:17">
-      <c r="A31" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2016</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
+      <c r="L31" s="1">
+        <v>1</v>
+      </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -2369,24 +2401,22 @@
     </row>
     <row r="32" ht="51" spans="1:17">
       <c r="A32" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B32" s="1">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1">
         <v>1</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="1">
-        <v>1</v>
-      </c>
+      <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1">
@@ -2395,21 +2425,23 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" ht="25.5" spans="1:17">
       <c r="A33" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B33" s="1">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2423,26 +2455,26 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" ht="52" customHeight="1" spans="1:17">
+    <row r="34" ht="51" spans="1:17">
       <c r="A34" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B34" s="1">
-        <v>2005</v>
+        <v>2013</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="F34" s="1"/>
       <c r="G34" s="1">
         <v>1</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="I34" s="1">
+        <v>1</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1">
@@ -2451,210 +2483,204 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" ht="51" spans="1:17">
+    <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B35" s="1">
-        <v>2007</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>2011</v>
+      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1">
-        <v>1</v>
-      </c>
+      <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
-      <c r="K35" s="1">
-        <v>1</v>
-      </c>
+      <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
-      <c r="O35" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" ht="63.75" spans="1:17">
+    <row r="36" ht="52" customHeight="1" spans="1:17">
       <c r="A36" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B36" s="1">
         <v>2005</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+        <v>129</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1">
-        <v>1</v>
-      </c>
+      <c r="L36" s="1">
+        <v>1</v>
+      </c>
+      <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" ht="51" spans="1:17">
       <c r="A37" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B37" s="1">
-        <v>2010</v>
-      </c>
-      <c r="C37" s="1"/>
+        <v>2007</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+      <c r="K37" s="1">
+        <v>1</v>
+      </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
+      <c r="O37" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" ht="25.5" spans="1:17">
+    <row r="38" ht="63.75" spans="1:17">
       <c r="A38" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B38" s="1">
-        <v>1991</v>
-      </c>
-      <c r="C38" s="1"/>
+        <v>2005</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="1">
-        <v>1</v>
-      </c>
+      <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
+      <c r="M38" s="1">
+        <v>1</v>
+      </c>
       <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
+      <c r="O38" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" ht="63.75" spans="1:13">
-      <c r="A39" t="s">
-        <v>133</v>
-      </c>
-      <c r="B39">
-        <v>2016</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-      <c r="M39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" ht="76.5" spans="1:17">
+    <row r="39" spans="1:17">
+      <c r="A39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2010</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+    </row>
+    <row r="40" ht="25.5" spans="1:17">
       <c r="A40" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B40" s="1">
-        <v>2016</v>
+        <v>1991</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="1">
-        <v>1</v>
-      </c>
+      <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
+      <c r="K40" s="1">
+        <v>1</v>
+      </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
-      <c r="O40" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-      <c r="Q40" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17">
-      <c r="A41" s="1" t="s">
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" ht="51" spans="1:13">
+      <c r="A41" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1">
-        <v>1</v>
-      </c>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1">
-        <v>1</v>
-      </c>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-    </row>
-    <row r="42" ht="51" spans="1:17">
+      <c r="B41">
+        <v>2016</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" ht="76.5" spans="1:17">
       <c r="A42" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B42" s="1">
         <v>2016</v>
@@ -2662,93 +2688,125 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="G42" s="1">
         <v>1</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="I42" s="1">
+        <v>1</v>
+      </c>
       <c r="J42" s="1"/>
-      <c r="K42" s="1">
-        <v>1</v>
-      </c>
+      <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="1">
-        <v>1</v>
-      </c>
+      <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" ht="38.25" spans="1:17">
-      <c r="A43" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B43" s="5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" ht="51" spans="1:17">
+      <c r="A43" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B43" s="1">
         <v>2016</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="1">
-        <v>1</v>
-      </c>
-      <c r="K43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1">
+        <v>1</v>
+      </c>
       <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
+      <c r="M43" s="1">
+        <v>1</v>
+      </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-    </row>
-    <row r="44" ht="38.25" spans="1:15">
-      <c r="A44" t="s">
-        <v>146</v>
-      </c>
-      <c r="B44">
+      <c r="Q43" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" ht="38.25" spans="1:17">
+      <c r="A44" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B44" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1">
+        <v>1</v>
+      </c>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+    </row>
+    <row r="45" ht="38.25" spans="1:15">
+      <c r="A45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45">
         <v>2014</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="45" ht="38.25" spans="1:5">
-      <c r="A45" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45">
+      <c r="E45" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" ht="38.25" spans="1:5">
+      <c r="A46" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46">
         <v>2008</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>149</v>
+      <c r="E46" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>